<commit_message>
Automake, ability to send requests to other servers, consistent hashing
</commit_message>
<xml_diff>
--- a/Performance.xlsx
+++ b/Performance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="152" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="109" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -100,7 +100,7 @@
     <t>128-2048</t>
   </si>
   <si>
-    <t>Both Cacheismo and memcached were given 1024 MB of RAM. </t>
+    <t>Both Cacheismo and memcached were given 1024 MB of RAM.</t>
   </si>
   <si>
     <t>Tests were run using the xmemcached client with 4 concurrent connections but varying number of threads and data size.</t>
@@ -610,11 +610,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="6230731"/>
-        <c:axId val="56747028"/>
+        <c:axId val="5989597"/>
+        <c:axId val="83075234"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="6230731"/>
+        <c:axId val="5989597"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -622,7 +622,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56747028"/>
+        <c:crossAx val="83075234"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -636,7 +636,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56747028"/>
+        <c:axId val="83075234"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -653,7 +653,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="6230731"/>
+        <c:crossAx val="5989597"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -695,10 +695,10 @@
       <xdr:rowOff>76320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>41400</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1477080</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -707,7 +707,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="89280" y="3639240"/>
-        <a:ext cx="9705240" cy="5096520"/>
+        <a:ext cx="9704880" cy="5096160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -732,14 +732,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5294117647059"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6392156862745"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8627450980392"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.2"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.556862745098"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.5254901960784"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.1294117647059"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="0" width="11.6745098039216"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6470588235294"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9607843137255"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.278431372549"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.6588235294118"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.643137254902"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.2352941176471"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="0" width="11.7294117647059"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -1314,7 +1314,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="0" width="11.6745098039216"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="0" width="11.7294117647059"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1339,7 +1339,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="0" width="11.6745098039216"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="0" width="11.7294117647059"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>